<commit_message>
Check IDataReader in DynamicPanel when render totals
</commit_message>
<xml_diff>
--- a/ExcelReporter.Tests/TestData/DataSourceDynamicPanelDataSetRenderTest/TestRenderDataSetWithEvents.xlsx
+++ b/ExcelReporter.Tests/TestData/DataSourceDynamicPanelDataSetRenderTest/TestRenderDataSetWithEvents.xlsx
@@ -781,7 +781,9 @@
       <x:c r="B6" s="10" t="n">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="C6" s="11" t="s"/>
+      <x:c r="C6" s="11" t="n">
+        <x:v>3</x:v>
+      </x:c>
       <x:c r="D6" s="11" t="s"/>
       <x:c r="E6" s="11" t="s"/>
       <x:c r="F6" s="11" t="s"/>

</xml_diff>